<commit_message>
more fiddling w model
</commit_message>
<xml_diff>
--- a/excel/2/1420 Terry - 2 - Add Taxes and Rent.xlsx
+++ b/excel/2/1420 Terry - 2 - Add Taxes and Rent.xlsx
@@ -3104,8 +3104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C96533-4FC3-8F4F-BA09-1D518A28119D}">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix typos in models
</commit_message>
<xml_diff>
--- a/excel/2/1420 Terry - 2 - Add Taxes and Rent.xlsx
+++ b/excel/2/1420 Terry - 2 - Add Taxes and Rent.xlsx
@@ -730,124 +730,124 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="1">
-                  <c:v>0.78397968171476839</c:v>
+                  <c:v>1.1804072389413525</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31300538416027812</c:v>
+                  <c:v>0.45796896088016137</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20938206279291893</c:v>
+                  <c:v>0.29902139086043084</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.16391290226085961</c:v>
+                  <c:v>0.22927826820476366</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13837403412515145</c:v>
+                  <c:v>0.19010685570056221</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12201978804482107</c:v>
+                  <c:v>0.16502404762501269</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1106524911462359</c:v>
+                  <c:v>0.14759090778577078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.10229421294428985</c:v>
+                  <c:v>0.13477342935143746</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11816583584190807</c:v>
+                  <c:v>0.1472296664907107</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11044697781133749</c:v>
+                  <c:v>0.13681179664279766</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.10419511329907022</c:v>
+                  <c:v>0.12837383371985236</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.902960380453428E-2</c:v>
+                  <c:v>0.12140205381852076</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.4690990790108315E-2</c:v>
+                  <c:v>0.11554628202951069</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.0996326816691356E-2</c:v>
+                  <c:v>0.11055960567362587</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.7812908812523544E-2</c:v>
+                  <c:v>0.10626292374256605</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5042137139123564E-2</c:v>
+                  <c:v>0.10252316249284442</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.2609221323316162E-2</c:v>
+                  <c:v>9.9239381918124356E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.0456402343204156E-2</c:v>
+                  <c:v>9.6333628293804902E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.8538365484940517E-2</c:v>
+                  <c:v>9.3744743197580999E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.6819059993795138E-2</c:v>
+                  <c:v>9.1424071192011305E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.5269446651487146E-2</c:v>
+                  <c:v>8.9332419870947713E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.3865872064305838E-2</c:v>
+                  <c:v>8.7437865738201725E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.2588875240473652E-2</c:v>
+                  <c:v>8.5714143519877453E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.1422298040783802E-2</c:v>
+                  <c:v>8.4139445595401485E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.0352612908637938E-2</c:v>
+                  <c:v>8.2695514676927206E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.9368408384038849E-2</c:v>
+                  <c:v>8.136694943984206E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.8459990823527619E-2</c:v>
+                  <c:v>8.014066698915083E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.7619072815309475E-2</c:v>
+                  <c:v>7.900548233291306E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.6838527043876911E-2</c:v>
+                  <c:v>7.7951776188762437E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.6112190107480831E-2</c:v>
+                  <c:v>7.697123020864996E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.5085920000000033E-2</c:v>
+                  <c:v>7.5707829333333379E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.5085920000000047E-2</c:v>
+                  <c:v>7.5707829333333393E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.5085920000000061E-2</c:v>
+                  <c:v>7.5707829333333407E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.5085920000000075E-2</c:v>
+                  <c:v>7.5707829333333421E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.5085920000000033E-2</c:v>
+                  <c:v>7.5707829333333365E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.5085920000000019E-2</c:v>
+                  <c:v>7.5707829333333351E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.5085920000000005E-2</c:v>
+                  <c:v>7.5707829333333337E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.5085920000000089E-2</c:v>
+                  <c:v>7.5707829333333435E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.5085920000000033E-2</c:v>
+                  <c:v>7.5707829333333365E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.5085920000000103E-2</c:v>
+                  <c:v>7.5707829333333435E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1333,127 +1333,127 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>-9683.8799999999974</c:v>
+                  <c:v>-6203.3999999999978</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-9338.9819999999963</c:v>
+                  <c:v>-5754.0875999999971</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8983.7370599999977</c:v>
+                  <c:v>-5291.2958279999948</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8617.8347717999932</c:v>
+                  <c:v>-4814.6203028399941</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-8240.9554149539981</c:v>
+                  <c:v>-4323.6445119252003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-7852.7696774026153</c:v>
+                  <c:v>-3817.9394472829499</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-7452.9383677246897</c:v>
+                  <c:v>-3297.0632307014366</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-7041.1121187564313</c:v>
+                  <c:v>-2760.5607276224819</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-6616.9310823191245</c:v>
+                  <c:v>-2207.9631494511541</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2699.5446147887014</c:v>
+                  <c:v>1841.6923560653067</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2249.5309532323663</c:v>
+                  <c:v>2427.9431267472664</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1786.0168818293369</c:v>
+                  <c:v>3031.7814205496834</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1308.5973882842118</c:v>
+                  <c:v>3653.7348631661735</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-816.85530993273824</c:v>
+                  <c:v>4294.3469090611597</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-310.36096923072</c:v>
+                  <c:v>4954.1773163329981</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>211.32820169235856</c:v>
+                  <c:v>5633.8026358229872</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>748.6680477431255</c:v>
+                  <c:v>6333.8167148976754</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1302.1280891754268</c:v>
+                  <c:v>7054.8312163446117</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1872.1919318506916</c:v>
+                  <c:v>7797.47615283495</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2459.3576898062111</c:v>
+                  <c:v>8562.4004374200013</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3064.1384205003906</c:v>
+                  <c:v>9350.2724505426013</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3687.0625731154087</c:v>
+                  <c:v>10161.78062405888</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4328.6744503088739</c:v>
+                  <c:v>10997.634042780646</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4989.5346838181376</c:v>
+                  <c:v>11858.563064064068</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5670.2207243326902</c:v>
+                  <c:v>12745.319955985995</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6371.3273460626697</c:v>
+                  <c:v>13658.679554665578</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7093.4671664445468</c:v>
+                  <c:v>14599.439941305542</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7837.2711814378818</c:v>
+                  <c:v>15568.423139544702</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8603.3893168810155</c:v>
+                  <c:v>16566.475833731045</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9392.4909963874379</c:v>
+                  <c:v>17594.470108742971</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10205.265726279062</c:v>
+                  <c:v>18653.304212005267</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>28742.423698067436</c:v>
+                  <c:v>37443.903338365424</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>29604.696409009463</c:v>
+                  <c:v>38567.220438516393</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>30492.837301279753</c:v>
+                  <c:v>39724.237051671887</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>31407.622420318141</c:v>
+                  <c:v>40915.964163222045</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>32349.851092927689</c:v>
+                  <c:v>42143.4430881187</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>33320.346625715523</c:v>
+                  <c:v>43407.74638076227</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>34319.957024486983</c:v>
+                  <c:v>44709.978772185132</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>35349.555735221598</c:v>
+                  <c:v>46051.278135350702</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>36410.042407278248</c:v>
+                  <c:v>47432.816479411216</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>37502.343679496596</c:v>
+                  <c:v>48855.800973793557</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3104,8 +3104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C96533-4FC3-8F4F-BA09-1D518A28119D}">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3186,8 +3186,8 @@
         <v>-290.04000000000002</v>
       </c>
       <c r="E2" s="5">
-        <f>-2062.95-C2</f>
-        <v>-587.94999999999982</v>
+        <f>-2062.95-C2-D2</f>
+        <v>-297.9099999999998</v>
       </c>
       <c r="F2" s="5">
         <v>-454</v>
@@ -3218,7 +3218,7 @@
       <c r="N2" s="11"/>
       <c r="O2" s="8">
         <f>12*(C2+D2+E2+F2+G2)</f>
-        <v>-9683.8799999999974</v>
+        <v>-6203.3999999999978</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -3237,7 +3237,7 @@
       </c>
       <c r="E3" s="5">
         <f>E2*(1+B3)</f>
-        <v>-605.58849999999984</v>
+        <v>-306.84729999999979</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F34" si="4">F2*(1+B3)</f>
@@ -3269,15 +3269,15 @@
       </c>
       <c r="M3" s="8">
         <f>L3-L2+12*(C3+D3+E3+F3+G3)</f>
-        <v>7089.528261746651</v>
+        <v>10674.42266174665</v>
       </c>
       <c r="N3" s="13">
         <f>M3/L2</f>
-        <v>0.78397968171476839</v>
+        <v>1.1804072389413525</v>
       </c>
       <c r="O3" s="8">
         <f t="shared" ref="O3:O66" si="6">12*(C3+D3+E3+F3+G3)</f>
-        <v>-9338.9819999999963</v>
+        <v>-5754.0875999999971</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -3296,7 +3296,7 @@
       </c>
       <c r="E4" s="5">
         <f t="shared" ref="E4:E67" si="7">E3*(1+B4)</f>
-        <v>-623.75615499999981</v>
+        <v>-316.0527189999998</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="4"/>
@@ -3328,15 +3328,15 @@
       </c>
       <c r="M4" s="8">
         <f t="shared" ref="M4:M67" si="9">L4-L3+12*(C4+D4+E4+F4+G4)</f>
-        <v>7972.7198546204763</v>
+        <v>11665.161086620479</v>
       </c>
       <c r="N4" s="13">
         <f t="shared" ref="N4:N67" si="10">M4/L3</f>
-        <v>0.31300538416027812</v>
+        <v>0.45796896088016137</v>
       </c>
       <c r="O4" s="8">
         <f t="shared" si="6"/>
-        <v>-8983.7370599999977</v>
+        <v>-5291.2958279999948</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -3355,7 +3355,7 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" si="7"/>
-        <v>-642.46883964999984</v>
+        <v>-325.5343005699998</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="4"/>
@@ -3387,15 +3387,15 @@
       </c>
       <c r="M5" s="8">
         <f t="shared" si="9"/>
-        <v>8883.6552874980043</v>
+        <v>12686.869756458003</v>
       </c>
       <c r="N5" s="13">
         <f t="shared" si="10"/>
-        <v>0.20938206279291893</v>
+        <v>0.29902139086043084</v>
       </c>
       <c r="O5" s="8">
         <f t="shared" si="6"/>
-        <v>-8617.8347717999932</v>
+        <v>-4814.6203028399941</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -3414,7 +3414,7 @@
       </c>
       <c r="E6" s="5">
         <f t="shared" si="7"/>
-        <v>-661.74290483949983</v>
+        <v>-335.30032958709978</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="4"/>
@@ -3446,15 +3446,15 @@
       </c>
       <c r="M6" s="8">
         <f t="shared" si="9"/>
-        <v>9823.2112664159431</v>
+        <v>13740.522169444741</v>
       </c>
       <c r="N6" s="13">
         <f t="shared" si="10"/>
-        <v>0.16391290226085961</v>
+        <v>0.22927826820476366</v>
       </c>
       <c r="O6" s="8">
         <f t="shared" si="6"/>
-        <v>-8240.9554149539981</v>
+        <v>-4323.6445119252003</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="E7" s="5">
         <f t="shared" si="7"/>
-        <v>-681.59519198468479</v>
+        <v>-345.35933947471278</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" si="4"/>
@@ -3505,15 +3505,15 @@
       </c>
       <c r="M7" s="8">
         <f t="shared" si="9"/>
-        <v>10792.292377440037</v>
+        <v>14827.122607559702</v>
       </c>
       <c r="N7" s="13">
         <f t="shared" si="10"/>
-        <v>0.13837403412515145</v>
+        <v>0.19010685570056221</v>
       </c>
       <c r="O7" s="8">
         <f t="shared" si="6"/>
-        <v>-7852.7696774026153</v>
+        <v>-3817.9394472829499</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -3533,7 +3533,7 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" si="7"/>
-        <v>-702.0430477442253</v>
+        <v>-355.72011965895416</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="4"/>
@@ -3565,15 +3565,15 @@
       </c>
       <c r="M8" s="8">
         <f t="shared" si="9"/>
-        <v>11791.831979218541</v>
+        <v>15947.707116241794</v>
       </c>
       <c r="N8" s="13">
         <f t="shared" si="10"/>
-        <v>0.12201978804482107</v>
+        <v>0.16502404762501269</v>
       </c>
       <c r="O8" s="8">
         <f t="shared" si="6"/>
-        <v>-7452.9383677246897</v>
+        <v>-3297.0632307014366</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="E9" s="5">
         <f t="shared" si="7"/>
-        <v>-723.10433917655212</v>
+        <v>-366.39172324872277</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="4"/>
@@ -3625,15 +3625,15 @@
       </c>
       <c r="M9" s="8">
         <f t="shared" si="9"/>
-        <v>12822.79312431355</v>
+        <v>17103.344515447498</v>
       </c>
       <c r="N9" s="13">
         <f t="shared" si="10"/>
-        <v>0.1106524911462359</v>
+        <v>0.14759090778577078</v>
       </c>
       <c r="O9" s="8">
         <f t="shared" si="6"/>
-        <v>-7041.1121187564313</v>
+        <v>-2760.5607276224819</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" si="7"/>
-        <v>-744.79746935184869</v>
+        <v>-377.38347494618444</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="4"/>
@@ -3685,15 +3685,15 @@
       </c>
       <c r="M10" s="8">
         <f t="shared" si="9"/>
-        <v>13886.169510237576</v>
+        <v>18295.137443105545</v>
       </c>
       <c r="N10" s="13">
         <f t="shared" si="10"/>
-        <v>0.10229421294428985</v>
+        <v>0.13477342935143746</v>
       </c>
       <c r="O10" s="8">
         <f t="shared" si="6"/>
-        <v>-6616.9310823191245</v>
+        <v>-2207.9631494511541</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="E11" s="5">
         <f t="shared" si="7"/>
-        <v>-767.14139343240413</v>
+        <v>-388.70497919457</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="4"/>
@@ -3745,15 +3745,15 @@
       </c>
       <c r="M11" s="8">
         <f t="shared" si="9"/>
-        <v>18463.466461164728</v>
+        <v>23004.703432018738</v>
       </c>
       <c r="N11" s="13">
         <f t="shared" si="10"/>
-        <v>0.11816583584190807</v>
+        <v>0.1472296664907107</v>
       </c>
       <c r="O11" s="8">
         <f t="shared" si="6"/>
-        <v>-2699.5446147887014</v>
+        <v>1841.6923560653067</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="E12" s="5">
         <f t="shared" si="7"/>
-        <v>-790.15563523537628</v>
+        <v>-400.36612857040711</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="4"/>
@@ -3805,15 +3805,15 @@
       </c>
       <c r="M12" s="8">
         <f t="shared" si="9"/>
-        <v>19594.781941310423</v>
+        <v>24272.256021290057</v>
       </c>
       <c r="N12" s="13">
         <f t="shared" si="10"/>
-        <v>0.11044697781133749</v>
+        <v>0.13681179664279766</v>
       </c>
       <c r="O12" s="8">
         <f t="shared" si="6"/>
-        <v>-2249.5309532323663</v>
+        <v>2427.9431267472664</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="E13" s="5">
         <f t="shared" si="7"/>
-        <v>-813.8603042924376</v>
+        <v>-412.37711242751936</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="4"/>
@@ -3865,15 +3865,15 @@
       </c>
       <c r="M13" s="8">
         <f t="shared" si="9"/>
-        <v>20761.687601010424</v>
+        <v>25579.485903389446</v>
       </c>
       <c r="N13" s="13">
         <f t="shared" si="10"/>
-        <v>0.10419511329907022</v>
+        <v>0.12837383371985236</v>
       </c>
       <c r="O13" s="8">
         <f t="shared" si="6"/>
-        <v>-1786.0168818293369</v>
+        <v>3031.7814205496834</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="E14" s="5">
         <f t="shared" si="7"/>
-        <v>-838.27611342121077</v>
+        <v>-424.74842580034493</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="4"/>
@@ -3925,15 +3925,15 @@
       </c>
       <c r="M14" s="8">
         <f t="shared" si="9"/>
-        <v>21965.309856559161</v>
+        <v>26927.642108009546</v>
       </c>
       <c r="N14" s="13">
         <f t="shared" si="10"/>
-        <v>9.902960380453428E-2</v>
+        <v>0.12140205381852076</v>
       </c>
       <c r="O14" s="8">
         <f t="shared" si="6"/>
-        <v>-1308.5973882842118</v>
+        <v>3653.7348631661735</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -3953,7 +3953,7 @@
       </c>
       <c r="E15" s="5">
         <f t="shared" si="7"/>
-        <v>-863.42439682384713</v>
+        <v>-437.49087857435529</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="4"/>
@@ -3985,15 +3985,15 @@
       </c>
       <c r="M15" s="8">
         <f t="shared" si="9"/>
-        <v>23206.811004908392</v>
+        <v>28318.013223902293</v>
       </c>
       <c r="N15" s="13">
         <f t="shared" si="10"/>
-        <v>9.4690990790108315E-2</v>
+        <v>0.11554628202951069</v>
       </c>
       <c r="O15" s="8">
         <f t="shared" si="6"/>
-        <v>-816.85530993273824</v>
+        <v>4294.3469090611597</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="E16" s="5">
         <f t="shared" si="7"/>
-        <v>-889.32712872856257</v>
+        <v>-450.61560493158595</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="4"/>
@@ -4045,15 +4045,15 @@
       </c>
       <c r="M16" s="8">
         <f t="shared" si="9"/>
-        <v>24487.390374355993</v>
+        <v>29751.928659919715</v>
       </c>
       <c r="N16" s="13">
         <f t="shared" si="10"/>
-        <v>9.0996326816691356E-2</v>
+        <v>0.11055960567362587</v>
       </c>
       <c r="O16" s="8">
         <f t="shared" si="6"/>
-        <v>-310.36096923072</v>
+        <v>4954.1773163329981</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="E17" s="5">
         <f t="shared" si="7"/>
-        <v>-916.0069425904195</v>
+        <v>-464.13407307953355</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="4"/>
@@ -4105,15 +4105,15 @@
       </c>
       <c r="M17" s="8">
         <f t="shared" si="9"/>
-        <v>25808.285512398561</v>
+        <v>31230.75994652919</v>
       </c>
       <c r="N17" s="13">
         <f t="shared" si="10"/>
-        <v>8.7812908812523544E-2</v>
+        <v>0.10626292374256605</v>
       </c>
       <c r="O17" s="8">
         <f t="shared" si="6"/>
-        <v>211.32820169235856</v>
+        <v>5633.8026358229872</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="E18" s="5">
         <f t="shared" si="7"/>
-        <v>-943.48715086813206</v>
+        <v>-478.05809527191957</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="4"/>
@@ -4165,15 +4165,15 @@
       </c>
       <c r="M18" s="8">
         <f t="shared" si="9"/>
-        <v>27170.773411952749</v>
+        <v>32755.922079107298</v>
       </c>
       <c r="N18" s="13">
         <f t="shared" si="10"/>
-        <v>8.5042137139123564E-2</v>
+        <v>0.10252316249284442</v>
       </c>
       <c r="O18" s="8">
         <f t="shared" si="6"/>
-        <v>748.6680477431255</v>
+        <v>6333.8167148976754</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="E19" s="5">
         <f t="shared" si="7"/>
-        <v>-971.79176539417608</v>
+        <v>-492.39983813007717</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="4"/>
@@ -4225,15 +4225,15 @@
       </c>
       <c r="M19" s="8">
         <f t="shared" si="9"/>
-        <v>28576.171777199415</v>
+        <v>34328.874904368597</v>
       </c>
       <c r="N19" s="13">
         <f t="shared" si="10"/>
-        <v>8.2609221323316162E-2</v>
+        <v>9.9239381918124356E-2</v>
       </c>
       <c r="O19" s="8">
         <f t="shared" si="6"/>
-        <v>1302.1280891754268</v>
+        <v>7054.8312163446117</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="E20" s="5">
         <f t="shared" si="7"/>
-        <v>-1000.9455183560013</v>
+        <v>-507.17183327397947</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="4"/>
@@ -4285,15 +4285,15 @@
       </c>
       <c r="M20" s="8">
         <f t="shared" si="9"/>
-        <v>30025.840330332408</v>
+        <v>35951.124551316665</v>
       </c>
       <c r="N20" s="13">
         <f t="shared" si="10"/>
-        <v>8.0456402343204156E-2</v>
+        <v>9.6333628293804902E-2</v>
       </c>
       <c r="O20" s="8">
         <f t="shared" si="6"/>
-        <v>1872.1919318506916</v>
+        <v>7797.47615283495</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="E21" s="5">
         <f t="shared" si="7"/>
-        <v>-1030.9738839066815</v>
+        <v>-522.38698827219889</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="4"/>
@@ -4345,15 +4345,15 @@
       </c>
       <c r="M21" s="8">
         <f t="shared" si="9"/>
-        <v>31521.182160552598</v>
+        <v>37624.22490816639</v>
       </c>
       <c r="N21" s="13">
         <f t="shared" si="10"/>
-        <v>7.8538365484940517E-2</v>
+        <v>9.3744743197580999E-2</v>
       </c>
       <c r="O21" s="8">
         <f t="shared" si="6"/>
-        <v>2459.3576898062111</v>
+        <v>8562.4004374200013</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="E22" s="5">
         <f t="shared" si="7"/>
-        <v>-1061.9031004238821</v>
+        <v>-538.05859792036483</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="4"/>
@@ -4405,15 +4405,15 @@
       </c>
       <c r="M22" s="8">
         <f t="shared" si="9"/>
-        <v>33063.645116672684</v>
+        <v>39349.779146714893</v>
       </c>
       <c r="N22" s="13">
         <f t="shared" si="10"/>
-        <v>7.6819059993795138E-2</v>
+        <v>9.1424071192011305E-2</v>
       </c>
       <c r="O22" s="8">
         <f t="shared" si="6"/>
-        <v>3064.1384205003906</v>
+        <v>9350.2724505426013</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -4433,7 +4433,7 @@
       </c>
       <c r="E23" s="5">
         <f t="shared" si="7"/>
-        <v>-1093.7601934365985</v>
+        <v>-554.20035585797575</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="4"/>
@@ -4465,15 +4465,15 @@
       </c>
       <c r="M23" s="8">
         <f t="shared" si="9"/>
-        <v>34654.723244762346</v>
+        <v>41129.441295705823</v>
       </c>
       <c r="N23" s="13">
         <f t="shared" si="10"/>
-        <v>7.5269446651487146E-2</v>
+        <v>8.9332419870947713E-2</v>
       </c>
       <c r="O23" s="8">
         <f t="shared" si="6"/>
-        <v>3687.0625731154087</v>
+        <v>10161.78062405888</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="E24" s="5">
         <f t="shared" si="7"/>
-        <v>-1126.5729992396964</v>
+        <v>-570.82636653371503</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="4"/>
@@ -4525,15 +4525,15 @@
       </c>
       <c r="M24" s="8">
         <f t="shared" si="9"/>
-        <v>36295.958272292657</v>
+        <v>42964.917864764429</v>
       </c>
       <c r="N24" s="13">
         <f t="shared" si="10"/>
-        <v>7.3865872064305838E-2</v>
+        <v>8.7437865738201725E-2</v>
       </c>
       <c r="O24" s="8">
         <f t="shared" si="6"/>
-        <v>4328.6744503088739</v>
+        <v>10997.634042780646</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="E25" s="5">
         <f t="shared" si="7"/>
-        <v>-1160.3701892168874</v>
+        <v>-587.95115752972652</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" si="4"/>
@@ -4585,15 +4585,15 @@
       </c>
       <c r="M25" s="8">
         <f t="shared" si="9"/>
-        <v>37988.941140302071</v>
+        <v>44857.969520548002</v>
       </c>
       <c r="N25" s="13">
         <f t="shared" si="10"/>
-        <v>7.2588875240473652E-2</v>
+        <v>8.5714143519877453E-2</v>
       </c>
       <c r="O25" s="8">
         <f t="shared" si="6"/>
-        <v>4989.5346838181376</v>
+        <v>11858.563064064068</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -4613,7 +4613,7 @@
       </c>
       <c r="E26" s="5">
         <f t="shared" si="7"/>
-        <v>-1195.1812948933941</v>
+        <v>-605.58969225561827</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" si="4"/>
@@ -4645,15 +4645,15 @@
       </c>
       <c r="M26" s="8">
         <f t="shared" si="9"/>
-        <v>39735.313585142569</v>
+        <v>46810.41281679587</v>
       </c>
       <c r="N26" s="13">
         <f t="shared" si="10"/>
-        <v>7.1422298040783802E-2</v>
+        <v>8.4139445595401485E-2</v>
       </c>
       <c r="O26" s="8">
         <f t="shared" si="6"/>
-        <v>5670.2207243326902</v>
+        <v>12745.319955985995</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="E27" s="5">
         <f t="shared" si="7"/>
-        <v>-1231.036733740196</v>
+        <v>-623.75738302328682</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="4"/>
@@ -4705,15 +4705,15 @@
       </c>
       <c r="M27" s="8">
         <f t="shared" si="9"/>
-        <v>41536.769771425199</v>
+        <v>48824.121980028111</v>
       </c>
       <c r="N27" s="13">
         <f t="shared" si="10"/>
-        <v>7.0352612908637938E-2</v>
+        <v>8.2695514676927206E-2</v>
       </c>
       <c r="O27" s="8">
         <f t="shared" si="6"/>
-        <v>6371.3273460626697</v>
+        <v>13658.679554665578</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="E28" s="5">
         <f t="shared" si="7"/>
-        <v>-1267.9678357524019</v>
+        <v>-642.47010451398546</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="4"/>
@@ -4765,15 +4765,15 @@
       </c>
       <c r="M28" s="8">
         <f t="shared" si="9"/>
-        <v>43395.057977836725</v>
+        <v>50901.030752697719</v>
       </c>
       <c r="N28" s="13">
         <f t="shared" si="10"/>
-        <v>6.9368408384038849E-2</v>
+        <v>8.136694943984206E-2</v>
       </c>
       <c r="O28" s="8">
         <f t="shared" si="6"/>
-        <v>7093.4671664445468</v>
+        <v>14599.439941305542</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="E29" s="5">
         <f t="shared" si="7"/>
-        <v>-1306.0068708249739</v>
+        <v>-661.7442076494051</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" si="4"/>
@@ -4825,15 +4825,15 @@
       </c>
       <c r="M29" s="8">
         <f t="shared" si="9"/>
-        <v>45311.982337543974</v>
+        <v>53043.134295650787</v>
       </c>
       <c r="N29" s="13">
         <f t="shared" si="10"/>
-        <v>6.8459990823527619E-2</v>
+        <v>8.014066698915083E-2</v>
       </c>
       <c r="O29" s="8">
         <f t="shared" si="6"/>
-        <v>7837.2711814378818</v>
+        <v>15568.423139544702</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="E30" s="5">
         <f t="shared" si="7"/>
-        <v>-1345.1870769497232</v>
+        <v>-681.59653387888727</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="4"/>
@@ -4885,15 +4885,15 @@
       </c>
       <c r="M30" s="8">
         <f t="shared" si="9"/>
-        <v>47289.404634975421</v>
+        <v>55252.491151825452</v>
       </c>
       <c r="N30" s="13">
         <f t="shared" si="10"/>
-        <v>6.7619072815309475E-2</v>
+        <v>7.900548233291306E-2</v>
       </c>
       <c r="O30" s="8">
         <f t="shared" si="6"/>
-        <v>8603.3893168810155</v>
+        <v>16566.475833731045</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="E31" s="5">
         <f t="shared" si="7"/>
-        <v>-1385.542689258215</v>
+        <v>-702.04442989525387</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" si="4"/>
@@ -4945,15 +4945,15 @@
       </c>
       <c r="M31" s="8">
         <f t="shared" si="9"/>
-        <v>49329.246160811745</v>
+        <v>57531.225273167278</v>
       </c>
       <c r="N31" s="13">
         <f t="shared" si="10"/>
-        <v>6.6838527043876911E-2</v>
+        <v>7.7951776188762437E-2</v>
       </c>
       <c r="O31" s="8">
         <f t="shared" si="6"/>
-        <v>9392.4909963874379</v>
+        <v>17594.470108742971</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -4973,7 +4973,7 @@
       </c>
       <c r="E32" s="5">
         <f t="shared" si="7"/>
-        <v>-1427.1089699359616</v>
+        <v>-723.10576279211148</v>
       </c>
       <c r="F32" s="5">
         <f t="shared" si="4"/>
@@ -5005,15 +5005,15 @@
       </c>
       <c r="M32" s="8">
         <f t="shared" si="9"/>
-        <v>51433.489627090807</v>
+        <v>59881.528112817017</v>
       </c>
       <c r="N32" s="13">
         <f t="shared" si="10"/>
-        <v>6.6112190107480831E-2</v>
+        <v>7.697123020864996E-2</v>
       </c>
       <c r="O32" s="8">
         <f t="shared" si="6"/>
-        <v>10205.265726279062</v>
+        <v>18653.304212005267</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -5032,7 +5032,7 @@
       </c>
       <c r="E33" s="5">
         <f t="shared" si="7"/>
-        <v>-1469.9222390340406</v>
+        <v>-744.79893567587487</v>
       </c>
       <c r="F33" s="5">
         <f t="shared" si="4"/>
@@ -5055,15 +5055,15 @@
       </c>
       <c r="M33" s="8">
         <f t="shared" si="9"/>
-        <v>53318.45621886279</v>
+        <v>62019.935859160782</v>
       </c>
       <c r="N33" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000033E-2</v>
+        <v>7.5707829333333379E-2</v>
       </c>
       <c r="O33" s="8">
         <f t="shared" si="6"/>
-        <v>28742.423698067436</v>
+        <v>37443.903338365424</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="E34" s="5">
         <f t="shared" si="7"/>
-        <v>-1514.0199062050617</v>
+        <v>-767.14290374615109</v>
       </c>
       <c r="F34" s="5">
         <f t="shared" si="4"/>
@@ -5105,15 +5105,15 @@
       </c>
       <c r="M34" s="8">
         <f t="shared" si="9"/>
-        <v>54918.009905428691</v>
+        <v>63880.533934935622</v>
       </c>
       <c r="N34" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000047E-2</v>
+        <v>7.5707829333333393E-2</v>
       </c>
       <c r="O34" s="8">
         <f t="shared" si="6"/>
-        <v>29604.696409009463</v>
+        <v>38567.220438516393</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -5132,7 +5132,7 @@
       </c>
       <c r="E35" s="5">
         <f t="shared" si="7"/>
-        <v>-1559.4405033912135</v>
+        <v>-790.15719085853561</v>
       </c>
       <c r="F35" s="5">
         <f t="shared" ref="F35:F71" si="12">F34*(1+B35)</f>
@@ -5155,15 +5155,15 @@
       </c>
       <c r="M35" s="8">
         <f t="shared" si="9"/>
-        <v>56565.550202591563</v>
+        <v>65796.949952983705</v>
       </c>
       <c r="N35" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000061E-2</v>
+        <v>7.5707829333333407E-2</v>
       </c>
       <c r="O35" s="8">
         <f t="shared" si="6"/>
-        <v>30492.837301279753</v>
+        <v>39724.237051671887</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -5182,7 +5182,7 @@
       </c>
       <c r="E36" s="5">
         <f t="shared" si="7"/>
-        <v>-1606.22371849295</v>
+        <v>-813.86190658429166</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" si="12"/>
@@ -5205,15 +5205,15 @@
       </c>
       <c r="M36" s="8">
         <f t="shared" si="9"/>
-        <v>58262.516708669318</v>
+        <v>67770.858451573222</v>
       </c>
       <c r="N36" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000075E-2</v>
+        <v>7.5707829333333421E-2</v>
       </c>
       <c r="O36" s="8">
         <f t="shared" si="6"/>
-        <v>31407.622420318141</v>
+        <v>40915.964163222045</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
@@ -5232,7 +5232,7 @@
       </c>
       <c r="E37" s="5">
         <f t="shared" si="7"/>
-        <v>-1654.4104300477386</v>
+        <v>-838.27776378182045</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" si="12"/>
@@ -5255,15 +5255,15 @@
       </c>
       <c r="M37" s="8">
         <f t="shared" si="9"/>
-        <v>60010.392209929363</v>
+        <v>69803.984205120374</v>
       </c>
       <c r="N37" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000033E-2</v>
+        <v>7.5707829333333365E-2</v>
       </c>
       <c r="O37" s="8">
         <f t="shared" si="6"/>
-        <v>32349.851092927689</v>
+        <v>42143.4430881187</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -5282,7 +5282,7 @@
       </c>
       <c r="E38" s="5">
         <f t="shared" si="7"/>
-        <v>-1704.0427429491708</v>
+        <v>-863.42609669527508</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" si="12"/>
@@ -5305,15 +5305,15 @@
       </c>
       <c r="M38" s="8">
         <f t="shared" si="9"/>
-        <v>61810.703976227232</v>
+        <v>71898.103731273979</v>
       </c>
       <c r="N38" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000019E-2</v>
+        <v>7.5707829333333351E-2</v>
       </c>
       <c r="O38" s="8">
         <f t="shared" si="6"/>
-        <v>33320.346625715523</v>
+        <v>43407.74638076227</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -5332,7 +5332,7 @@
       </c>
       <c r="E39" s="5">
         <f t="shared" si="7"/>
-        <v>-1755.164025237646</v>
+        <v>-889.32887959613333</v>
       </c>
       <c r="F39" s="5">
         <f t="shared" si="12"/>
@@ -5355,15 +5355,15 @@
       </c>
       <c r="M39" s="8">
         <f t="shared" si="9"/>
-        <v>63665.025095514036</v>
+        <v>74055.046843212185</v>
       </c>
       <c r="N39" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000005E-2</v>
+        <v>7.5707829333333337E-2</v>
       </c>
       <c r="O39" s="8">
         <f t="shared" si="6"/>
-        <v>34319.957024486983</v>
+        <v>44709.978772185132</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -5382,7 +5382,7 @@
       </c>
       <c r="E40" s="5">
         <f t="shared" si="7"/>
-        <v>-1807.8189459947755</v>
+        <v>-916.00874598401731</v>
       </c>
       <c r="F40" s="5">
         <f t="shared" si="12"/>
@@ -5405,15 +5405,15 @@
       </c>
       <c r="M40" s="8">
         <f t="shared" si="9"/>
-        <v>65574.975848379545</v>
+        <v>76276.698248508648</v>
       </c>
       <c r="N40" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000089E-2</v>
+        <v>7.5707829333333435E-2</v>
       </c>
       <c r="O40" s="8">
         <f t="shared" si="6"/>
-        <v>35349.555735221598</v>
+        <v>46051.278135350702</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -5432,7 +5432,7 @@
       </c>
       <c r="E41" s="5">
         <f t="shared" si="7"/>
-        <v>-1862.0535143746188</v>
+        <v>-943.48900836353789</v>
       </c>
       <c r="F41" s="5">
         <f t="shared" si="12"/>
@@ -5455,15 +5455,15 @@
       </c>
       <c r="M41" s="8">
         <f t="shared" si="9"/>
-        <v>67542.225123830882</v>
+        <v>78564.999195963843</v>
       </c>
       <c r="N41" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000033E-2</v>
+        <v>7.5707829333333365E-2</v>
       </c>
       <c r="O41" s="8">
         <f t="shared" si="6"/>
-        <v>36410.042407278248</v>
+        <v>47432.816479411216</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -5482,7 +5482,7 @@
       </c>
       <c r="E42" s="5">
         <f t="shared" si="7"/>
-        <v>-1917.9151198058573</v>
+        <v>-971.79367861444405</v>
       </c>
       <c r="F42" s="5">
         <f t="shared" si="12"/>
@@ -5505,15 +5505,15 @@
       </c>
       <c r="M42" s="8">
         <f t="shared" si="9"/>
-        <v>69568.491877545879</v>
+        <v>80921.949171842833</v>
       </c>
       <c r="N42" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000103E-2</v>
+        <v>7.5707829333333435E-2</v>
       </c>
       <c r="O42" s="8">
         <f t="shared" si="6"/>
-        <v>37502.343679496596</v>
+        <v>48855.800973793557</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -5532,7 +5532,7 @@
       </c>
       <c r="E43" s="5">
         <f t="shared" si="7"/>
-        <v>-1975.4525734000331</v>
+        <v>-1000.9474889728774</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="12"/>
@@ -5555,15 +5555,15 @@
       </c>
       <c r="M43" s="8">
         <f t="shared" si="9"/>
-        <v>71655.546633872174</v>
+        <v>83349.607646998047</v>
       </c>
       <c r="N43" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000019E-2</v>
+        <v>7.5707829333333365E-2</v>
       </c>
       <c r="O43" s="8">
         <f t="shared" si="6"/>
-        <v>38627.41398988149</v>
+        <v>50321.475003007363</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -5582,7 +5582,7 @@
       </c>
       <c r="E44" s="5">
         <f t="shared" si="7"/>
-        <v>-2034.7161506020341</v>
+        <v>-1030.9759136420637</v>
       </c>
       <c r="F44" s="5">
         <f t="shared" si="12"/>
@@ -5605,15 +5605,15 @@
       </c>
       <c r="M44" s="8">
         <f t="shared" si="9"/>
-        <v>73805.213032888409</v>
+        <v>85850.095876408057</v>
       </c>
       <c r="N44" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000075E-2</v>
+        <v>7.5707829333333421E-2</v>
       </c>
       <c r="O44" s="8">
         <f t="shared" si="6"/>
-        <v>39786.236409577934</v>
+        <v>51831.119253097582</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -5632,7 +5632,7 @@
       </c>
       <c r="E45" s="5">
         <f t="shared" si="7"/>
-        <v>-2095.7576351200951</v>
+        <v>-1061.9051910513256</v>
       </c>
       <c r="F45" s="5">
         <f t="shared" si="12"/>
@@ -5655,15 +5655,15 @@
       </c>
       <c r="M45" s="8">
         <f t="shared" si="9"/>
-        <v>76019.369423875018</v>
+        <v>88425.598752700258</v>
       </c>
       <c r="N45" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000033E-2</v>
+        <v>7.5707829333333379E-2</v>
       </c>
       <c r="O45" s="8">
         <f t="shared" si="6"/>
-        <v>40979.823501865278</v>
+        <v>53386.052830690518</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -5682,7 +5682,7 @@
       </c>
       <c r="E46" s="5">
         <f t="shared" si="7"/>
-        <v>-2158.6303641736981</v>
+        <v>-1093.7623467828653</v>
       </c>
       <c r="F46" s="5">
         <f t="shared" si="12"/>
@@ -5705,15 +5705,15 @@
       </c>
       <c r="M46" s="8">
         <f t="shared" si="9"/>
-        <v>78299.950506591354</v>
+        <v>91078.366715281343</v>
       </c>
       <c r="N46" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000103E-2</v>
+        <v>7.5707829333333448E-2</v>
       </c>
       <c r="O46" s="8">
         <f t="shared" si="6"/>
-        <v>42209.218206921243</v>
+        <v>54987.634415611232</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
@@ -5732,7 +5732,7 @@
       </c>
       <c r="E47" s="5">
         <f t="shared" si="7"/>
-        <v>-2223.3892750989089</v>
+        <v>-1126.5752171863512</v>
       </c>
       <c r="F47" s="5">
         <f t="shared" si="12"/>
@@ -5755,15 +5755,15 @@
       </c>
       <c r="M47" s="8">
         <f t="shared" si="9"/>
-        <v>80648.949021789042</v>
+        <v>93810.717716739746</v>
       </c>
       <c r="N47" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000061E-2</v>
+        <v>7.5707829333333407E-2</v>
       </c>
       <c r="O47" s="8">
         <f t="shared" si="6"/>
-        <v>43475.494753128885</v>
+        <v>56637.263448079582</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -5782,7 +5782,7 @@
       </c>
       <c r="E48" s="5">
         <f t="shared" si="7"/>
-        <v>-2290.0909533518761</v>
+        <v>-1160.3724737019418</v>
       </c>
       <c r="F48" s="5">
         <f t="shared" si="12"/>
@@ -5805,15 +5805,15 @@
       </c>
       <c r="M48" s="8">
         <f t="shared" si="9"/>
-        <v>83068.417492442633</v>
+        <v>96625.039248241839</v>
       </c>
       <c r="N48" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085919999999992E-2</v>
+        <v>7.5707829333333324E-2</v>
       </c>
       <c r="O48" s="8">
         <f t="shared" si="6"/>
-        <v>44779.75959572276</v>
+        <v>58336.381351521966</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
@@ -5832,7 +5832,7 @@
       </c>
       <c r="E49" s="5">
         <f t="shared" si="7"/>
-        <v>-2358.7936819524325</v>
+        <v>-1195.183647913</v>
       </c>
       <c r="F49" s="5">
         <f t="shared" si="12"/>
@@ -5855,15 +5855,15 @@
       </c>
       <c r="M49" s="8">
         <f t="shared" si="9"/>
-        <v>85560.470017216066</v>
+        <v>99523.790425689251</v>
       </c>
       <c r="N49" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000103E-2</v>
+        <v>7.5707829333333448E-2</v>
       </c>
       <c r="O49" s="8">
         <f t="shared" si="6"/>
-        <v>46123.152383594439</v>
+        <v>60086.472792067631</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
@@ -5882,7 +5882,7 @@
       </c>
       <c r="E50" s="5">
         <f t="shared" si="7"/>
-        <v>-2429.5574924110056</v>
+        <v>-1231.03915735039</v>
       </c>
       <c r="F50" s="5">
         <f t="shared" si="12"/>
@@ -5905,15 +5905,15 @@
       </c>
       <c r="M50" s="8">
         <f t="shared" si="9"/>
-        <v>88127.284117732517</v>
+        <v>102509.50413845992</v>
       </c>
       <c r="N50" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000075E-2</v>
+        <v>7.5707829333333435E-2</v>
       </c>
       <c r="O50" s="8">
         <f t="shared" si="6"/>
-        <v>47506.846955102264</v>
+        <v>61889.066975829657</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
@@ -5932,7 +5932,7 @@
       </c>
       <c r="E51" s="5">
         <f t="shared" si="7"/>
-        <v>-2502.4442171833357</v>
+        <v>-1267.9703320709018</v>
       </c>
       <c r="F51" s="5">
         <f t="shared" si="12"/>
@@ -5955,15 +5955,15 @@
       </c>
       <c r="M51" s="8">
         <f t="shared" si="9"/>
-        <v>90771.10264126437</v>
+        <v>105584.78926261357</v>
       </c>
       <c r="N51" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085919999999978E-2</v>
+        <v>7.5707829333333324E-2</v>
       </c>
       <c r="O51" s="8">
         <f t="shared" si="6"/>
-        <v>48932.052363755342</v>
+        <v>63745.738985104545</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
@@ -5982,7 +5982,7 @@
       </c>
       <c r="E52" s="5">
         <f t="shared" si="7"/>
-        <v>-2577.5175436988357</v>
+        <v>-1306.0094420330288</v>
       </c>
       <c r="F52" s="5">
         <f t="shared" si="12"/>
@@ -6005,15 +6005,15 @@
       </c>
       <c r="M52" s="8">
         <f t="shared" si="9"/>
-        <v>93494.2357205023</v>
+        <v>108752.33294049196</v>
       </c>
       <c r="N52" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085919999999978E-2</v>
+        <v>7.570782933333331E-2</v>
       </c>
       <c r="O52" s="8">
         <f t="shared" si="6"/>
-        <v>50400.013934668001</v>
+        <v>65658.111154657672</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
@@ -6032,7 +6032,7 @@
       </c>
       <c r="E53" s="5">
         <f t="shared" si="7"/>
-        <v>-2654.8430700098006</v>
+        <v>-1345.1897252940196</v>
       </c>
       <c r="F53" s="5">
         <f t="shared" si="12"/>
@@ -6055,15 +6055,15 @@
       </c>
       <c r="M53" s="8">
         <f t="shared" si="9"/>
-        <v>96299.062792117387</v>
+        <v>112014.90292870675</v>
       </c>
       <c r="N53" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085919999999992E-2</v>
+        <v>7.5707829333333337E-2</v>
       </c>
       <c r="O53" s="8">
         <f t="shared" si="6"/>
-        <v>51912.014352708036</v>
+        <v>67627.854489297402</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
@@ -6082,7 +6082,7 @@
       </c>
       <c r="E54" s="5">
         <f t="shared" si="7"/>
-        <v>-2734.4883621100948</v>
+        <v>-1385.5454170528401</v>
       </c>
       <c r="F54" s="5">
         <f t="shared" si="12"/>
@@ -6105,15 +6105,15 @@
       </c>
       <c r="M54" s="8">
         <f t="shared" si="9"/>
-        <v>99188.034675880917</v>
+        <v>115375.35001656797</v>
       </c>
       <c r="N54" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000005E-2</v>
+        <v>7.5707829333333337E-2</v>
       </c>
       <c r="O54" s="8">
         <f t="shared" si="6"/>
-        <v>53469.37478328927</v>
+        <v>69656.690123976325</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
@@ -6132,7 +6132,7 @@
       </c>
       <c r="E55" s="5">
         <f t="shared" si="7"/>
-        <v>-2816.5230129733977</v>
+        <v>-1427.1117795644254</v>
       </c>
       <c r="F55" s="5">
         <f t="shared" si="12"/>
@@ -6155,15 +6155,15 @@
       </c>
       <c r="M55" s="8">
         <f t="shared" si="9"/>
-        <v>102163.67571615739</v>
+        <v>118836.61051706504</v>
       </c>
       <c r="N55" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000033E-2</v>
+        <v>7.5707829333333365E-2</v>
       </c>
       <c r="O55" s="8">
         <f t="shared" si="6"/>
-        <v>55073.45602678795</v>
+        <v>71746.390827695606</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
@@ -6182,7 +6182,7 @@
       </c>
       <c r="E56" s="5">
         <f t="shared" si="7"/>
-        <v>-2901.0187033625998</v>
+        <v>-1469.9251329513581</v>
       </c>
       <c r="F56" s="5">
         <f t="shared" si="12"/>
@@ -6205,15 +6205,15 @@
       </c>
       <c r="M56" s="8">
         <f t="shared" si="9"/>
-        <v>105228.58598764212</v>
+        <v>122401.70883257702</v>
       </c>
       <c r="N56" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000033E-2</v>
+        <v>7.5707829333333379E-2</v>
       </c>
       <c r="O56" s="8">
         <f t="shared" si="6"/>
-        <v>56725.659707591578</v>
+        <v>73898.782552526478</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
@@ -6232,7 +6232,7 @@
       </c>
       <c r="E57" s="5">
         <f t="shared" si="7"/>
-        <v>-2988.0492644634778</v>
+        <v>-1514.0228869398989</v>
       </c>
       <c r="F57" s="5">
         <f t="shared" si="12"/>
@@ -6255,15 +6255,15 @@
       </c>
       <c r="M57" s="8">
         <f t="shared" si="9"/>
-        <v>108385.44356727127</v>
+        <v>126073.76009755422</v>
       </c>
       <c r="N57" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085919999999964E-2</v>
+        <v>7.570782933333331E-2</v>
       </c>
       <c r="O57" s="8">
         <f t="shared" si="6"/>
-        <v>58427.429498819329</v>
+        <v>76115.746029102273</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
@@ -6282,7 +6282,7 @@
       </c>
       <c r="E58" s="5">
         <f t="shared" si="7"/>
-        <v>-3077.6907423973821</v>
+        <v>-1559.4435735480959</v>
       </c>
       <c r="F58" s="5">
         <f t="shared" si="12"/>
@@ -6305,15 +6305,15 @@
       </c>
       <c r="M58" s="8">
         <f t="shared" si="9"/>
-        <v>111637.0068742896</v>
+        <v>129855.97290048102</v>
       </c>
       <c r="N58" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000075E-2</v>
+        <v>7.5707829333333407E-2</v>
       </c>
       <c r="O58" s="8">
         <f t="shared" si="6"/>
-        <v>60180.252383783925</v>
+        <v>78399.21840997535</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -6332,7 +6332,7 @@
       </c>
       <c r="E59" s="5">
         <f t="shared" si="7"/>
-        <v>-3170.0214646693034</v>
+        <v>-1606.2268807545388</v>
       </c>
       <c r="F59" s="5">
         <f t="shared" si="12"/>
@@ -6355,15 +6355,15 @@
       </c>
       <c r="M59" s="8">
         <f t="shared" si="9"/>
-        <v>114986.11708051813</v>
+        <v>133751.65208749531</v>
       </c>
       <c r="N59" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085919999999978E-2</v>
+        <v>7.5707829333333324E-2</v>
       </c>
       <c r="O59" s="8">
         <f t="shared" si="6"/>
-        <v>61985.659955297451</v>
+        <v>80751.194962274632</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
@@ -6382,7 +6382,7 @@
       </c>
       <c r="E60" s="5">
         <f t="shared" si="7"/>
-        <v>-3265.1221086093828</v>
+        <v>-1654.413687177175</v>
       </c>
       <c r="F60" s="5">
         <f t="shared" si="12"/>
@@ -6405,15 +6405,15 @@
       </c>
       <c r="M60" s="8">
         <f t="shared" si="9"/>
-        <v>118435.70059293386</v>
+        <v>137764.20165012038</v>
       </c>
       <c r="N60" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000089E-2</v>
+        <v>7.5707829333333435E-2</v>
       </c>
       <c r="O60" s="8">
         <f t="shared" si="6"/>
-        <v>63845.229753956366</v>
+        <v>83173.730811142872</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
@@ -6432,7 +6432,7 @@
       </c>
       <c r="E61" s="5">
         <f t="shared" si="7"/>
-        <v>-3363.0757718676646</v>
+        <v>-1704.0460977924904</v>
       </c>
       <c r="F61" s="5">
         <f t="shared" si="12"/>
@@ -6455,15 +6455,15 @@
       </c>
       <c r="M61" s="8">
         <f t="shared" si="9"/>
-        <v>121988.77161072177</v>
+        <v>141897.12769962384</v>
       </c>
       <c r="N61" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000019E-2</v>
+        <v>7.5707829333333351E-2</v>
       </c>
       <c r="O61" s="8">
         <f t="shared" si="6"/>
-        <v>65760.586646575073</v>
+        <v>85668.942735477147</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
@@ -6482,7 +6482,7 @@
       </c>
       <c r="E62" s="5">
         <f t="shared" si="7"/>
-        <v>-3463.9680450236947</v>
+        <v>-1755.1674807262652</v>
       </c>
       <c r="F62" s="5">
         <f t="shared" si="12"/>
@@ -6505,15 +6505,15 @@
       </c>
       <c r="M62" s="8">
         <f t="shared" si="9"/>
-        <v>125648.4347590433</v>
+        <v>146154.04153061245</v>
       </c>
       <c r="N62" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085919999999964E-2</v>
+        <v>7.5707829333333296E-2</v>
       </c>
       <c r="O62" s="8">
         <f t="shared" si="6"/>
-        <v>67733.404245972313</v>
+        <v>88239.011017541474</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="E63" s="5">
         <f t="shared" si="7"/>
-        <v>-3567.8870863744055</v>
+        <v>-1807.8225051480533</v>
       </c>
       <c r="F63" s="5">
         <f t="shared" si="12"/>
@@ -6555,15 +6555,15 @@
       </c>
       <c r="M63" s="8">
         <f t="shared" si="9"/>
-        <v>129417.88780181474</v>
+        <v>150538.66277653095</v>
       </c>
       <c r="N63" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000033E-2</v>
+        <v>7.5707829333333365E-2</v>
       </c>
       <c r="O63" s="8">
         <f t="shared" si="6"/>
-        <v>69765.406373351492</v>
+        <v>90886.181348067708</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
@@ -6582,7 +6582,7 @@
       </c>
       <c r="E64" s="5">
         <f t="shared" si="7"/>
-        <v>-3674.9236989656379</v>
+        <v>-1862.057180302495</v>
       </c>
       <c r="F64" s="5">
         <f t="shared" si="12"/>
@@ -6605,15 +6605,15 @@
       </c>
       <c r="M64" s="8">
         <f t="shared" si="9"/>
-        <v>133300.42443586921</v>
+        <v>155054.82265982692</v>
       </c>
       <c r="N64" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000047E-2</v>
+        <v>7.5707829333333379E-2</v>
       </c>
       <c r="O64" s="8">
         <f t="shared" si="6"/>
-        <v>71858.368564552031</v>
+        <v>93612.766788509762</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
@@ -6632,7 +6632,7 @@
       </c>
       <c r="E65" s="5">
         <f t="shared" si="7"/>
-        <v>-3785.1714099346073</v>
+        <v>-1917.9188957115698</v>
       </c>
       <c r="F65" s="5">
         <f t="shared" si="12"/>
@@ -6655,15 +6655,15 @@
       </c>
       <c r="M65" s="8">
         <f t="shared" si="9"/>
-        <v>137299.43716894541</v>
+        <v>159706.46733962186</v>
       </c>
       <c r="N65" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085920000000103E-2</v>
+        <v>7.5707829333333435E-2</v>
       </c>
       <c r="O65" s="8">
         <f t="shared" si="6"/>
-        <v>74014.119621488586</v>
+        <v>96421.149792165044</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
@@ -6682,7 +6682,7 @@
       </c>
       <c r="E66" s="5">
         <f t="shared" si="7"/>
-        <v>-3898.7265522326456</v>
+        <v>-1975.4564625829169</v>
       </c>
       <c r="F66" s="5">
         <f t="shared" si="12"/>
@@ -6705,15 +6705,15 @@
       </c>
       <c r="M66" s="8">
         <f t="shared" si="9"/>
-        <v>141418.42028401355</v>
+        <v>164497.66135981027</v>
       </c>
       <c r="N66" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085919999999992E-2</v>
+        <v>7.5707829333333324E-2</v>
       </c>
       <c r="O66" s="8">
         <f t="shared" si="6"/>
-        <v>76234.54321013327</v>
+        <v>99313.78428593</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
@@ -6732,7 +6732,7 @@
       </c>
       <c r="E67" s="5">
         <f t="shared" si="7"/>
-        <v>-4015.6883487996251</v>
+        <v>-2034.7201564604045</v>
       </c>
       <c r="F67" s="5">
         <f t="shared" si="12"/>
@@ -6755,15 +6755,15 @@
       </c>
       <c r="M67" s="8">
         <f t="shared" si="9"/>
-        <v>145660.97289253396</v>
+        <v>169432.5912006046</v>
       </c>
       <c r="N67" s="13">
         <f t="shared" si="10"/>
-        <v>6.5085919999999992E-2</v>
+        <v>7.5707829333333324E-2</v>
       </c>
       <c r="O67" s="8">
         <f t="shared" ref="O67:O71" si="15">12*(C67+D67+E67+F67+G67)</f>
-        <v>78521.579506437265</v>
+        <v>102293.1978145079</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
@@ -6782,7 +6782,7 @@
       </c>
       <c r="E68" s="5">
         <f t="shared" ref="E68:E71" si="16">E67*(1+B68)</f>
-        <v>-4136.1589992636136</v>
+        <v>-2095.7617611542169</v>
       </c>
       <c r="F68" s="5">
         <f t="shared" si="12"/>
@@ -6805,15 +6805,15 @@
       </c>
       <c r="M68" s="8">
         <f t="shared" ref="M68:M71" si="18">L68-L67+12*(C68+D68+E68+F68+G68)</f>
-        <v>150030.80207931023</v>
+        <v>174515.56893662299</v>
       </c>
       <c r="N68" s="13">
         <f t="shared" ref="N68:N71" si="19">M68/L67</f>
-        <v>6.5085920000000103E-2</v>
+        <v>7.5707829333333435E-2</v>
       </c>
       <c r="O68" s="8">
         <f t="shared" si="15"/>
-        <v>80877.226891630387</v>
+        <v>105361.99374894313</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
@@ -6832,7 +6832,7 @@
       </c>
       <c r="E69" s="5">
         <f t="shared" si="16"/>
-        <v>-4260.2437692415224</v>
+        <v>-2158.6346139888433</v>
       </c>
       <c r="F69" s="5">
         <f t="shared" si="12"/>
@@ -6855,15 +6855,15 @@
       </c>
       <c r="M69" s="8">
         <f t="shared" si="18"/>
-        <v>154531.72614168935</v>
+        <v>179751.03600472148</v>
       </c>
       <c r="N69" s="13">
         <f t="shared" si="19"/>
-        <v>6.5085920000000019E-2</v>
+        <v>7.5707829333333351E-2</v>
       </c>
       <c r="O69" s="8">
         <f t="shared" si="15"/>
-        <v>83303.543698379304</v>
+        <v>108522.85356141144</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
@@ -6882,7 +6882,7 @@
       </c>
       <c r="E70" s="5">
         <f t="shared" si="16"/>
-        <v>-4388.0510823187678</v>
+        <v>-2223.3936524085088</v>
       </c>
       <c r="F70" s="5">
         <f t="shared" si="12"/>
@@ -6905,15 +6905,15 @@
       </c>
       <c r="M70" s="8">
         <f t="shared" si="18"/>
-        <v>159167.67792593996</v>
+        <v>185143.56708486308</v>
       </c>
       <c r="N70" s="13">
         <f t="shared" si="19"/>
-        <v>6.5085919999999992E-2</v>
+        <v>7.5707829333333324E-2</v>
       </c>
       <c r="O70" s="8">
         <f t="shared" si="15"/>
-        <v>85802.650009330668</v>
+        <v>111778.53916825377</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
@@ -6932,7 +6932,7 @@
       </c>
       <c r="E71" s="5">
         <f t="shared" si="16"/>
-        <v>-4519.6926147883314</v>
+        <v>-2290.095461980764</v>
       </c>
       <c r="F71" s="5">
         <f t="shared" si="12"/>
@@ -6955,15 +6955,15 @@
       </c>
       <c r="M71" s="8">
         <f t="shared" si="18"/>
-        <v>163942.70826371844</v>
+        <v>190697.87409740925</v>
       </c>
       <c r="N71" s="13">
         <f t="shared" si="19"/>
-        <v>6.5085920000000089E-2</v>
+        <v>7.5707829333333435E-2</v>
       </c>
       <c r="O71" s="8">
         <f t="shared" si="15"/>
-        <v>88376.729509610595</v>
+        <v>115131.89534330141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>